<commit_message>
# All Modules work.
* There were problems in loading "Progress" and "Scatter data" to load.
* In Progress, the coord_flip() does not work for ggpltly now. Take it off
</commit_message>
<xml_diff>
--- a/Files/Data_P2.xlsx
+++ b/Files/Data_P2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ardalanmirshani/Dropbox/RAAVI/RAAVI/Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ardalanmirshani/Dropbox/OCC/Shiny Templates/Shiny apps/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="24260" windowHeight="11860" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22440" windowHeight="11860"/>
   </bookViews>
   <sheets>
     <sheet name="ریاضی" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t/>
   </si>
@@ -64,7 +64,40 @@
     <t>10-25</t>
   </si>
   <si>
+    <t>رضا مولایی</t>
+  </si>
+  <si>
+    <t>محمود وکیلی</t>
+  </si>
+  <si>
     <t>علی شمس</t>
+  </si>
+  <si>
+    <t>رضا برهانی مرند</t>
+  </si>
+  <si>
+    <t>سینا وکیلی</t>
+  </si>
+  <si>
+    <t>رضا خوشخو</t>
+  </si>
+  <si>
+    <t>کسری نیک فرجام</t>
+  </si>
+  <si>
+    <t>سید محسن ابطحی</t>
+  </si>
+  <si>
+    <t>ندا اشرفی</t>
+  </si>
+  <si>
+    <t>اکرم سینایی</t>
+  </si>
+  <si>
+    <t>پوریا مقدسی</t>
+  </si>
+  <si>
+    <t>احمد رضا معین</t>
   </si>
   <si>
     <t>رضا سراب</t>
@@ -430,14 +463,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A2:A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -476,7 +506,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>15.6</v>
@@ -511,7 +541,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>18</v>
@@ -546,7 +576,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>17.5</v>
@@ -581,7 +611,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>15.7</v>
@@ -616,7 +646,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>16.8</v>
@@ -651,7 +681,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>18</v>
@@ -686,7 +716,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>18.100000000000001</v>
@@ -721,7 +751,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>19.100000000000001</v>
@@ -756,7 +786,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <v>15.5</v>
@@ -791,7 +821,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B11">
         <v>18.600000000000001</v>
@@ -826,7 +856,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B12">
         <v>15.5</v>
@@ -861,7 +891,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <v>17.600000000000001</v>
@@ -904,14 +934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -950,7 +975,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>18.2</v>
@@ -985,7 +1010,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>17.100000000000001</v>
@@ -1020,7 +1045,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>15.5</v>
@@ -1378,14 +1403,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1424,7 +1444,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>18.100000000000001</v>
@@ -1459,7 +1479,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>18</v>
@@ -1494,7 +1514,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>17.899999999999999</v>

</xml_diff>